<commit_message>
Updated measurements excel files
</commit_message>
<xml_diff>
--- a/Measurements/Test 3 - No obstacles VamiaV0/Statistics3.xlsx
+++ b/Measurements/Test 3 - No obstacles VamiaV0/Statistics3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\CodeFromGithub\SerialPortRead\Vamia-SerialPortReading\Measurements\Test 3 - No obstacles VamiaV0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\code\SerialReading\Measurements\Test 3 - No obstacles VamiaV0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C02FA5C-D65A-4AB4-8D72-741F848937B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7AB0E8-BF6B-4AA1-9D44-1D4485350F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1269,16 +1267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1591,15 +1589,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1613,7 +1611,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1634,8 +1632,15 @@
         <f>10*$G$1*LOG(A2/100, 10)+$F$1</f>
         <v>#NUM!</v>
       </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>POWER(10,(E2-$F$1)/(10*$G$1))*100</f>
+        <v>10.895694104353964</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -1656,8 +1661,15 @@
         <f t="shared" ref="F3:F21" si="1">10*$G$1*LOG(A3/100, 10)+$F$1</f>
         <v>43.817509926287684</v>
       </c>
+      <c r="H3" s="1">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I21" si="2">POWER(10,(E3-$F$1)/(10*$G$1))*100</f>
+        <v>13.170669235432172</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>40</v>
       </c>
@@ -1678,8 +1690,15 @@
         <f t="shared" si="1"/>
         <v>48.935019852575365</v>
       </c>
+      <c r="H4" s="1">
+        <v>40</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>14.677992676220683</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -1700,8 +1719,15 @@
         <f t="shared" si="1"/>
         <v>51.928571256521948</v>
       </c>
+      <c r="H5" s="1">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>55.352501822582809</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>80</v>
       </c>
@@ -1722,8 +1748,15 @@
         <f t="shared" si="1"/>
         <v>54.052529778863047</v>
       </c>
+      <c r="H6" s="1">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>100.4525080125163</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100</v>
       </c>
@@ -1744,8 +1777,15 @@
         <f t="shared" si="1"/>
         <v>55.7</v>
       </c>
+      <c r="H7" s="1">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>45.791441345065806</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>120</v>
       </c>
@@ -1766,8 +1806,15 @@
         <f t="shared" si="1"/>
         <v>57.046081182809623</v>
       </c>
+      <c r="H8" s="1">
+        <v>120</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>96.889008090955741</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>140</v>
       </c>
@@ -1788,8 +1835,15 @@
         <f t="shared" si="1"/>
         <v>58.184176606530052</v>
       </c>
+      <c r="H9" s="1">
+        <v>140</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>111.94884258038485</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>160</v>
       </c>
@@ -1810,8 +1864,15 @@
         <f t="shared" si="1"/>
         <v>59.170039705150728</v>
       </c>
+      <c r="H10" s="1">
+        <v>160</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>132.90135589851747</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>180</v>
       </c>
@@ -1832,8 +1893,15 @@
         <f t="shared" si="1"/>
         <v>60.039632586756206</v>
       </c>
+      <c r="H11" s="1">
+        <v>180</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>239.01842072885051</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>200</v>
       </c>
@@ -1854,8 +1922,15 @@
         <f t="shared" si="1"/>
         <v>60.817509926287684</v>
       </c>
+      <c r="H12" s="1">
+        <v>200</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>352.41860156398235</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>240</v>
       </c>
@@ -1876,8 +1951,15 @@
         <f t="shared" si="1"/>
         <v>62.163591109097304</v>
       </c>
+      <c r="H13" s="1">
+        <v>240</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>205.00511914680786</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>280</v>
       </c>
@@ -1898,8 +1980,15 @@
         <f t="shared" si="1"/>
         <v>63.301686532817726</v>
       </c>
+      <c r="H14" s="1">
+        <v>280</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>313.38516308650213</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>320</v>
       </c>
@@ -1920,8 +2009,15 @@
         <f t="shared" si="1"/>
         <v>64.287549631438409</v>
       </c>
+      <c r="H15" s="1">
+        <v>320</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>327.85836933913055</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>360</v>
       </c>
@@ -1942,8 +2038,15 @@
         <f t="shared" si="1"/>
         <v>65.15714251304388</v>
       </c>
+      <c r="H16" s="1">
+        <v>360</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>281.20277870087114</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>400</v>
       </c>
@@ -1964,8 +2067,15 @@
         <f t="shared" si="1"/>
         <v>65.935019852575365</v>
       </c>
+      <c r="H17" s="1">
+        <v>400</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>276.16998133438477</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>440</v>
       </c>
@@ -1986,8 +2096,15 @@
         <f t="shared" si="1"/>
         <v>66.638695500265186</v>
       </c>
+      <c r="H18" s="1">
+        <v>440</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>382.25479435982811</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>480</v>
       </c>
@@ -2008,8 +2125,15 @@
         <f t="shared" si="1"/>
         <v>67.281101035384978</v>
       </c>
+      <c r="H19" s="1">
+        <v>480</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>358.84091944691147</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>520</v>
       </c>
@@ -2030,8 +2154,15 @@
         <f t="shared" si="1"/>
         <v>67.87205684179159</v>
       </c>
+      <c r="H20" s="1">
+        <v>520</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>579.08871012454449</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>560</v>
       </c>
@@ -2051,6 +2182,13 @@
       <c r="F21">
         <f t="shared" si="1"/>
         <v>68.419196459105407</v>
+      </c>
+      <c r="H21" s="1">
+        <v>560</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>519.62049765698896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>